<commit_message>
Actualización definición páginas formulario #18
Se modifica el documento al haberse detectado errores (formularios que no son necesarios).
</commit_message>
<xml_diff>
--- a/Documentación Soporte/Definición de páginas de formulario.xlsx
+++ b/Documentación Soporte/Definición de páginas de formulario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\UBU\TFG\_Documentos proyecto\Modelado de Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\GitHub\TFG.-Desarrollo-de-un-Sistema-de-Planificacion-y-Gestion-de-la-Contratacion-Publica-2021-22\Documentación Soporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3856F0C6-EE4F-462E-BC42-362A120C1A21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F53287-B867-4013-8B0F-A010BA6B7FB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" xr2:uid="{DECAB956-C519-4D79-AE5B-A2E6ADF22B94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="138">
   <si>
     <t>Global Page - Desktop</t>
   </si>
@@ -106,15 +106,6 @@
   </si>
   <si>
     <t>Edición Previsiones</t>
-  </si>
-  <si>
-    <t>Aplicaciones presupuestarias previsiones</t>
-  </si>
-  <si>
-    <t>Imputaciones presupuestarias</t>
-  </si>
-  <si>
-    <t>Distribución Previsión</t>
   </si>
   <si>
     <t>Eventos Planificación</t>
@@ -808,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E83957-F1F0-4864-B048-D7F9308C9178}">
-  <dimension ref="A1:C134"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D113" sqref="D2:D113"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1037,7 +1028,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1048,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1056,43 +1047,43 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>208</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>209</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>210</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>280</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1100,10 +1091,10 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>300</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1111,10 +1102,10 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>301</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1122,10 +1113,10 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>302</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1133,10 +1124,10 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>340</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1144,10 +1135,10 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C30">
-        <v>341</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1155,10 +1146,10 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>370</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1166,10 +1157,10 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>371</v>
+        <v>401</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1177,10 +1168,10 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>380</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1188,10 +1179,10 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>400</v>
+        <v>432</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1199,10 +1190,10 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C35">
-        <v>401</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1210,43 +1201,43 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <v>431</v>
+        <v>500</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>432</v>
+        <v>501</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>480</v>
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
       <c r="C39">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1257,7 +1248,7 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>501</v>
+        <v>601</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1268,7 +1259,7 @@
         <v>8</v>
       </c>
       <c r="C41">
-        <v>502</v>
+        <v>602</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1279,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="C42">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1290,7 +1281,7 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>601</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1301,62 +1292,62 @@
         <v>8</v>
       </c>
       <c r="C44">
-        <v>602</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C45">
-        <v>1000</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>1101</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C47">
-        <v>1102</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>1111</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>1112</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1364,43 +1355,43 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>1121</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>1122</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C52">
-        <v>1131</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C53">
-        <v>1132</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1408,43 +1399,43 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54">
-        <v>1141</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>1142</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C56">
-        <v>1151</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>1152</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1452,10 +1443,10 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C58">
-        <v>1201</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1463,10 +1454,10 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>1202</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1474,10 +1465,10 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60">
-        <v>1211</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1485,10 +1476,10 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>1212</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1496,65 +1487,65 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C62">
-        <v>1221</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>1222</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C64">
-        <v>1231</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C65">
-        <v>1232</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C66">
-        <v>1241</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>1242</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1562,10 +1553,10 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C68">
-        <v>1301</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1573,10 +1564,10 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C69">
-        <v>1302</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1584,10 +1575,10 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>1311</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1595,10 +1586,10 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>1312</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1606,10 +1597,10 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>1321</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1617,10 +1608,10 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>1322</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1628,10 +1619,10 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C74">
-        <v>1331</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1639,10 +1630,10 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C75">
-        <v>1332</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1650,10 +1641,10 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C76">
-        <v>1341</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1661,10 +1652,10 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C77">
-        <v>1342</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1672,10 +1663,10 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>1351</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1683,10 +1674,10 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C79">
-        <v>1352</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1694,10 +1685,10 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C80">
-        <v>1361</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1705,10 +1696,10 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C81">
-        <v>1362</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1716,10 +1707,10 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C82">
-        <v>1371</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1727,10 +1718,10 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C83">
-        <v>1372</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1738,10 +1729,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C84">
-        <v>1381</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1749,10 +1740,10 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>1382</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1760,43 +1751,43 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C86">
-        <v>1391</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>1392</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C88">
-        <v>1401</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C89">
-        <v>1402</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1804,10 +1795,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C90">
-        <v>1501</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -1815,10 +1806,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>1502</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1826,10 +1817,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C92">
-        <v>1511</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1837,10 +1828,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>1512</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1848,10 +1839,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>1521</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1859,10 +1850,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C95">
-        <v>1522</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1870,10 +1861,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>1531</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1881,10 +1872,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C97">
-        <v>1532</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -1892,10 +1883,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C98">
-        <v>1541</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1903,10 +1894,10 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C99">
-        <v>1542</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -1914,10 +1905,10 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C100">
-        <v>1551</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -1925,10 +1916,10 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C101">
-        <v>1552</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -1936,10 +1927,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C102">
-        <v>1561</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -1947,10 +1938,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C103">
-        <v>1562</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -1958,10 +1949,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C104">
-        <v>1571</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -1969,10 +1960,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C105">
-        <v>1572</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -1980,10 +1971,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C106">
-        <v>1581</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -1991,10 +1982,10 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C107">
-        <v>1582</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -2002,10 +1993,10 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C108">
-        <v>1601</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -2013,10 +2004,10 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>1602</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -2024,98 +2015,98 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C110">
-        <v>1611</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B111" t="s">
         <v>8</v>
       </c>
       <c r="C111">
-        <v>1612</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="C112">
-        <v>1701</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="C113">
-        <v>1702</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C114">
-        <v>5000</v>
+        <v>10010</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C115">
-        <v>9999</v>
+        <v>10020</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C116">
-        <v>10000</v>
+        <v>10030</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
       </c>
       <c r="C117">
-        <v>10010</v>
+        <v>10031</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>10020</v>
+        <v>10032</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -2123,10 +2114,10 @@
         <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="C119">
-        <v>10030</v>
+        <v>10033</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -2137,7 +2128,7 @@
         <v>6</v>
       </c>
       <c r="C120">
-        <v>10031</v>
+        <v>10034</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -2145,10 +2136,10 @@
         <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="C121">
-        <v>10032</v>
+        <v>10040</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -2159,40 +2150,40 @@
         <v>6</v>
       </c>
       <c r="C122">
-        <v>10033</v>
+        <v>10041</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C123">
-        <v>10034</v>
+        <v>10042</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C124">
-        <v>10040</v>
+        <v>10043</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="C125">
-        <v>10041</v>
+        <v>10044</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -2200,10 +2191,10 @@
         <v>131</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="C126">
-        <v>10042</v>
+        <v>10050</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -2211,32 +2202,32 @@
         <v>132</v>
       </c>
       <c r="B127" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C127">
-        <v>10043</v>
+        <v>10051</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="C128">
-        <v>10044</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C129">
-        <v>10050</v>
+        <v>10054</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -2244,59 +2235,26 @@
         <v>135</v>
       </c>
       <c r="B130" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C130">
-        <v>10051</v>
+        <v>10060</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
+        <v>136</v>
+      </c>
+      <c r="B131" t="s">
         <v>137</v>
       </c>
-      <c r="B131" t="s">
-        <v>6</v>
-      </c>
       <c r="C131">
-        <v>10053</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
-        <v>134</v>
-      </c>
-      <c r="B132" t="s">
-        <v>124</v>
-      </c>
-      <c r="C132">
-        <v>10054</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
-        <v>138</v>
-      </c>
-      <c r="B133" t="s">
-        <v>136</v>
-      </c>
-      <c r="C133">
-        <v>10060</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
-        <v>139</v>
-      </c>
-      <c r="B134" t="s">
-        <v>140</v>
-      </c>
-      <c r="C134">
         <v>10061</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D134">
-    <sortCondition ref="C1:C134"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D131">
+    <sortCondition ref="C1:C131"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>